<commit_message>
cn-#18 Ignore cells after two empty cells.
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/BasicSample.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/BasicSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0010ACE5-0A94-445B-AE4C-E6124E5B6C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4138256E-C05B-47CA-9665-D9509D4673D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_intro" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Scenario</t>
   </si>
@@ -61,9 +61,6 @@
     <t>When</t>
   </si>
   <si>
-    <t>the two numbers are added</t>
-  </si>
-  <si>
     <t>Then</t>
   </si>
   <si>
@@ -77,6 +74,18 @@
   </si>
   <si>
     <t>This is a sample file to test Cactus.net</t>
+  </si>
+  <si>
+    <t>Cells after two empty space will be ignored.</t>
+  </si>
+  <si>
+    <t>the two numbers are</t>
+  </si>
+  <si>
+    <t>added</t>
+  </si>
+  <si>
+    <t>ignored</t>
   </si>
 </sst>
 </file>
@@ -396,7 +405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3737E3-24AF-4942-8F66-F45EBA2F7056}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -404,7 +413,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -414,66 +423,78 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <f>C2+C3</f>
+      <c r="C7">
+        <f>C3+C4</f>
         <v>120</v>
       </c>
     </row>
@@ -500,7 +521,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -530,15 +551,15 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
       </c>
       <c r="C6">
         <f>C2-C3</f>

</xml_diff>